<commit_message>
Se crea una tabla de bitacora de carga
</commit_message>
<xml_diff>
--- a/database/Database_Dictionary.xlsx
+++ b/database/Database_Dictionary.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Columns" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Columns!$B$2:$I$147</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Columns!$B$2:$I$154</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="165">
   <si>
     <t>DATABASE_NAME</t>
   </si>
@@ -134,6 +134,12 @@
     <t>Temporary table of travel transactions</t>
   </si>
   <si>
+    <t>DIM_LOG_CARGA</t>
+  </si>
+  <si>
+    <t>Dimensional table of the load log</t>
+  </si>
+  <si>
     <t>VIEW</t>
   </si>
   <si>
@@ -462,6 +468,48 @@
   </si>
   <si>
     <t>nvarchar</t>
+  </si>
+  <si>
+    <t>FCH_LOG</t>
+  </si>
+  <si>
+    <t>Log date</t>
+  </si>
+  <si>
+    <t>ID_PROCESO</t>
+  </si>
+  <si>
+    <t>ID of the process</t>
+  </si>
+  <si>
+    <t>NOM_ARCHIVO</t>
+  </si>
+  <si>
+    <t>File name to upload</t>
+  </si>
+  <si>
+    <t>REGISTROS_NOM_ARCHIVO</t>
+  </si>
+  <si>
+    <t>Number of records in the file</t>
+  </si>
+  <si>
+    <t>NOM_TABLA</t>
+  </si>
+  <si>
+    <t>Table of the table to load</t>
+  </si>
+  <si>
+    <t>REGISTROS_INSERTADOS_TABLA</t>
+  </si>
+  <si>
+    <t>Number of records loaded into the table</t>
+  </si>
+  <si>
+    <t>COMENTARIO</t>
+  </si>
+  <si>
+    <t>Comment about upload</t>
   </si>
   <si>
     <t>Fee amount</t>
@@ -1635,7 +1683,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:F24"/>
+  <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1928,16 +1976,16 @@
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -1945,7 +1993,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>41</v>
@@ -1962,7 +2010,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>43</v>
@@ -1979,7 +2027,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>45</v>
@@ -1996,7 +2044,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>47</v>
@@ -2013,7 +2061,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>49</v>
@@ -2030,7 +2078,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>51</v>
@@ -2040,6 +2088,23 @@
       </c>
       <c r="F24" s="1" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2051,7 +2116,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:I147"/>
+  <dimension ref="B2:I154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2063,7 +2128,7 @@
     <col min="3" max="3" width="15.5714285714286" customWidth="1"/>
     <col min="4" max="4" width="31.1428571428571" customWidth="1"/>
     <col min="5" max="5" width="17.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="25.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="32.2857142857143" customWidth="1"/>
     <col min="7" max="7" width="14.2857142857143" customWidth="1"/>
     <col min="8" max="8" width="15.7142857142857" customWidth="1"/>
     <col min="9" max="9" width="47.2857142857143" customWidth="1"/>
@@ -2083,13 +2148,13 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>4</v>
@@ -2109,16 +2174,16 @@
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H3" s="1">
         <v>4</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:9">
@@ -2135,16 +2200,16 @@
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H4" s="1">
         <v>8</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -2161,16 +2226,16 @@
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="H5" s="1">
         <v>8</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -2187,16 +2252,16 @@
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H6" s="1">
         <v>4</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -2213,16 +2278,16 @@
         <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H7" s="1">
         <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -2239,16 +2304,16 @@
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H8" s="1">
         <v>8</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -2265,16 +2330,16 @@
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H9" s="1">
         <v>4</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -2291,16 +2356,16 @@
         <v>8</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H10" s="1">
         <v>50</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -2317,16 +2382,16 @@
         <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H11" s="1">
         <v>4</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="2:9">
@@ -2343,16 +2408,16 @@
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H12" s="1">
         <v>50</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="2:9">
@@ -2369,16 +2434,16 @@
         <v>8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H13" s="1">
         <v>4</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="2:9">
@@ -2395,16 +2460,16 @@
         <v>8</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H14" s="1">
         <v>50</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="2:9">
@@ -2421,16 +2486,16 @@
         <v>8</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H15" s="1">
         <v>4</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:9">
@@ -2447,16 +2512,16 @@
         <v>8</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H16" s="1">
         <v>30</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="2:9">
@@ -2473,16 +2538,16 @@
         <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H17" s="1">
         <v>3</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="2:9">
@@ -2499,16 +2564,16 @@
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H18" s="1">
         <v>4</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:9">
@@ -2525,16 +2590,16 @@
         <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H19" s="1">
         <v>4</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="2:9">
@@ -2551,16 +2616,16 @@
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H20" s="1">
         <v>4</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="2:9">
@@ -2577,16 +2642,16 @@
         <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H21" s="1">
         <v>4</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="2:9">
@@ -2603,16 +2668,16 @@
         <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H22" s="1">
         <v>12</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="2:9">
@@ -2629,16 +2694,16 @@
         <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H23" s="1">
         <v>4</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="2:9">
@@ -2655,16 +2720,16 @@
         <v>8</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H24" s="1">
         <v>4</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="2:9">
@@ -2681,16 +2746,16 @@
         <v>8</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H25" s="1">
         <v>30</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="2:9">
@@ -2707,16 +2772,16 @@
         <v>8</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H26" s="1">
         <v>3</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="2:9">
@@ -2733,16 +2798,16 @@
         <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H27" s="1">
         <v>4</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="2:9">
@@ -2759,16 +2824,16 @@
         <v>8</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H28" s="1">
         <v>4</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="2:9">
@@ -2785,16 +2850,16 @@
         <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H29" s="1">
         <v>4</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="2:9">
@@ -2811,16 +2876,16 @@
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H30" s="1">
         <v>4</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="2:9">
@@ -2837,16 +2902,16 @@
         <v>8</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H31" s="1">
         <v>12</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="2:9">
@@ -2863,16 +2928,16 @@
         <v>8</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H32" s="1">
         <v>4</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="2:9">
@@ -2889,16 +2954,16 @@
         <v>8</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H33" s="1">
         <v>4</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="2:9">
@@ -2915,16 +2980,16 @@
         <v>8</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H34" s="1">
         <v>12</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="2:9">
@@ -2941,16 +3006,16 @@
         <v>8</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H35" s="1">
         <v>4</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="2:9">
@@ -2967,16 +3032,16 @@
         <v>8</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H36" s="1">
         <v>4</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="2:9">
@@ -2993,16 +3058,16 @@
         <v>8</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H37" s="1">
         <v>4</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="2:9">
@@ -3019,16 +3084,16 @@
         <v>8</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H38" s="1">
         <v>4</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="2:9">
@@ -3045,16 +3110,16 @@
         <v>8</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H39" s="1">
         <v>4</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="2:9">
@@ -3071,16 +3136,16 @@
         <v>8</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H40" s="1">
         <v>4</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="2:9">
@@ -3097,16 +3162,16 @@
         <v>8</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H41" s="1">
         <v>4</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="2:9">
@@ -3123,16 +3188,16 @@
         <v>8</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H42" s="1">
         <v>4</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="2:9">
@@ -3149,16 +3214,16 @@
         <v>8</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H43" s="1">
         <v>8</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="2:9">
@@ -3175,16 +3240,16 @@
         <v>8</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H44" s="1">
         <v>5</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="2:9">
@@ -3201,16 +3266,16 @@
         <v>8</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H45" s="1">
         <v>8</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="2:9">
@@ -3227,16 +3292,16 @@
         <v>8</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H46" s="1">
         <v>8</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="2:9">
@@ -3253,16 +3318,16 @@
         <v>8</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H47" s="1">
         <v>8</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="2:9">
@@ -3279,16 +3344,16 @@
         <v>8</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H48" s="1">
         <v>8</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="2:9">
@@ -3305,16 +3370,16 @@
         <v>8</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H49" s="1">
         <v>8</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="2:9">
@@ -3331,16 +3396,16 @@
         <v>8</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H50" s="1">
         <v>8</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="2:9">
@@ -3357,16 +3422,16 @@
         <v>8</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H51" s="1">
         <v>8</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="2:9">
@@ -3383,16 +3448,16 @@
         <v>8</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H52" s="1">
         <v>8</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="2:9">
@@ -3409,16 +3474,16 @@
         <v>8</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="H53" s="1">
         <v>8</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="2:9">
@@ -3435,16 +3500,16 @@
         <v>8</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H54" s="1">
         <v>8</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="2:9">
@@ -3461,16 +3526,16 @@
         <v>8</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H55" s="1">
         <v>8</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="2:9">
@@ -3487,16 +3552,16 @@
         <v>8</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H56" s="1">
         <v>4</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="2:9">
@@ -3513,16 +3578,16 @@
         <v>8</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H57" s="1">
         <v>-1</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="2:9">
@@ -3539,16 +3604,16 @@
         <v>8</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H58" s="1">
         <v>4</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="2:9">
@@ -3565,16 +3630,16 @@
         <v>8</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H59" s="1">
         <v>-1</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="2:9">
@@ -3591,16 +3656,16 @@
         <v>8</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H60" s="1">
         <v>4</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="2:9">
@@ -3617,16 +3682,16 @@
         <v>8</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H61" s="1">
         <v>-1</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="2:9">
@@ -3643,16 +3708,16 @@
         <v>8</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H62" s="1">
         <v>-1</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="2:9">
@@ -3669,16 +3734,16 @@
         <v>8</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H63" s="1">
         <v>-1</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="2:9">
@@ -3695,16 +3760,16 @@
         <v>8</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H64" s="1">
         <v>4</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="2:9">
@@ -3721,16 +3786,16 @@
         <v>8</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H65" s="1">
         <v>4</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="2:9">
@@ -3747,16 +3812,16 @@
         <v>8</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H66" s="1">
         <v>4</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="2:9">
@@ -3773,16 +3838,16 @@
         <v>8</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H67" s="1">
         <v>4</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="2:9">
@@ -3799,16 +3864,16 @@
         <v>8</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H68" s="1">
         <v>4</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="2:9">
@@ -3825,16 +3890,16 @@
         <v>8</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H69" s="1">
         <v>4</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="2:9">
@@ -3851,16 +3916,16 @@
         <v>8</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H70" s="1">
         <v>4</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="2:9">
@@ -3877,16 +3942,16 @@
         <v>8</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H71" s="1">
         <v>8</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="72" spans="2:9">
@@ -3903,16 +3968,16 @@
         <v>8</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H72" s="1">
         <v>-1</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="2:9">
@@ -3929,16 +3994,16 @@
         <v>8</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H73" s="1">
         <v>8</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="2:9">
@@ -3955,16 +4020,16 @@
         <v>8</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H74" s="1">
         <v>8</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="2:9">
@@ -3981,16 +4046,16 @@
         <v>8</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H75" s="1">
         <v>8</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76" spans="2:9">
@@ -4007,16 +4072,16 @@
         <v>8</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H76" s="1">
         <v>8</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="2:9">
@@ -4033,16 +4098,16 @@
         <v>8</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H77" s="1">
         <v>8</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="78" spans="2:9">
@@ -4059,16 +4124,16 @@
         <v>8</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H78" s="1">
         <v>8</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="2:9">
@@ -4085,16 +4150,16 @@
         <v>8</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H79" s="1">
         <v>8</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="2:9">
@@ -4111,16 +4176,16 @@
         <v>8</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H80" s="1">
         <v>4</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="81" spans="2:9">
@@ -4137,16 +4202,16 @@
         <v>8</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H81" s="1">
         <v>-1</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="2:9">
@@ -4163,16 +4228,16 @@
         <v>8</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H82" s="1">
         <v>-1</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="2:9">
@@ -4189,16 +4254,16 @@
         <v>8</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H83" s="1">
         <v>4</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="2:9">
@@ -4215,16 +4280,16 @@
         <v>8</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H84" s="1">
         <v>8</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="2:9">
@@ -4241,16 +4306,16 @@
         <v>8</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H85" s="1">
         <v>8</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="2:9">
@@ -4267,16 +4332,16 @@
         <v>8</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H86" s="1">
         <v>8</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="87" spans="2:9">
@@ -4293,16 +4358,16 @@
         <v>8</v>
       </c>
       <c r="F87" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G87" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G87" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="H87" s="1">
         <v>8</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="88" spans="2:9">
@@ -4319,16 +4384,16 @@
         <v>8</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H88" s="1">
         <v>4</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="89" spans="2:9">
@@ -4345,16 +4410,16 @@
         <v>8</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H89" s="1">
         <v>4</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="2:9">
@@ -4371,16 +4436,16 @@
         <v>8</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H90" s="1">
         <v>8</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="91" spans="2:9">
@@ -4397,16 +4462,16 @@
         <v>8</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H91" s="1">
         <v>-1</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="92" spans="2:9">
@@ -4423,16 +4488,16 @@
         <v>8</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H92" s="1">
         <v>8</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="93" spans="2:9">
@@ -4449,16 +4514,16 @@
         <v>8</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H93" s="1">
         <v>8</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="94" spans="2:9">
@@ -4475,16 +4540,16 @@
         <v>8</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H94" s="1">
         <v>8</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="95" spans="2:9">
@@ -4501,16 +4566,16 @@
         <v>8</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H95" s="1">
         <v>8</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="96" spans="2:9">
@@ -4527,16 +4592,16 @@
         <v>8</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H96" s="1">
         <v>8</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="97" spans="2:9">
@@ -4553,16 +4618,16 @@
         <v>8</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H97" s="1">
         <v>8</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" spans="2:9">
@@ -4579,16 +4644,16 @@
         <v>8</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H98" s="1">
         <v>8</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="99" spans="2:9">
@@ -4596,25 +4661,25 @@
         <v>5</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E99" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>57</v>
+        <v>149</v>
       </c>
       <c r="H99" s="1">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>58</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" spans="2:9">
@@ -4622,25 +4687,25 @@
         <v>5</v>
       </c>
       <c r="C100" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E100" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H100" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>61</v>
+        <v>153</v>
       </c>
     </row>
     <row r="101" spans="2:9">
@@ -4648,25 +4713,25 @@
         <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E101" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>62</v>
+        <v>154</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>60</v>
+        <v>149</v>
       </c>
       <c r="H101" s="1">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>63</v>
+        <v>155</v>
       </c>
     </row>
     <row r="102" spans="2:9">
@@ -4674,25 +4739,25 @@
         <v>5</v>
       </c>
       <c r="C102" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E102" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>64</v>
+        <v>156</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H102" s="1">
         <v>4</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
     </row>
     <row r="103" spans="2:9">
@@ -4700,25 +4765,25 @@
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E103" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>66</v>
+        <v>158</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>60</v>
+        <v>149</v>
       </c>
       <c r="H103" s="1">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>67</v>
+        <v>159</v>
       </c>
     </row>
     <row r="104" spans="2:9">
@@ -4726,25 +4791,25 @@
         <v>5</v>
       </c>
       <c r="C104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E104" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>68</v>
+        <v>160</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H104" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>69</v>
+        <v>161</v>
       </c>
     </row>
     <row r="105" spans="2:9">
@@ -4752,25 +4817,25 @@
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D105" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="E105" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>70</v>
+        <v>162</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H105" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>71</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="2:9">
@@ -4778,25 +4843,25 @@
         <v>5</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H106" s="1">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="107" spans="2:9">
@@ -4804,25 +4869,25 @@
         <v>5</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H107" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="108" spans="2:9">
@@ -4830,25 +4895,25 @@
         <v>5</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H108" s="1">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="109" spans="2:9">
@@ -4856,25 +4921,25 @@
         <v>5</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H109" s="1">
         <v>4</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="110" spans="2:9">
@@ -4882,25 +4947,25 @@
         <v>5</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H110" s="1">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="2:9">
@@ -4908,25 +4973,25 @@
         <v>5</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H111" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="112" spans="2:9">
@@ -4934,25 +4999,25 @@
         <v>5</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="G112" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H112" s="1">
+        <v>4</v>
+      </c>
+      <c r="I112" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="H112" s="1">
-        <v>30</v>
-      </c>
-      <c r="I112" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="113" spans="2:9">
@@ -4960,25 +5025,25 @@
         <v>5</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="H113" s="1">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="114" spans="2:9">
@@ -4986,25 +5051,25 @@
         <v>5</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H114" s="1">
         <v>4</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="115" spans="2:9">
@@ -5012,25 +5077,25 @@
         <v>5</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="H115" s="1">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="116" spans="2:9">
@@ -5038,7 +5103,7 @@
         <v>5</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>49</v>
@@ -5047,16 +5112,16 @@
         <v>8</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H116" s="1">
         <v>4</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="117" spans="2:9">
@@ -5064,7 +5129,7 @@
         <v>5</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>49</v>
@@ -5073,16 +5138,16 @@
         <v>8</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="H117" s="1">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="118" spans="2:9">
@@ -5090,25 +5155,25 @@
         <v>5</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H118" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="119" spans="2:9">
@@ -5116,25 +5181,25 @@
         <v>5</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="H119" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="120" spans="2:9">
@@ -5142,25 +5207,25 @@
         <v>5</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H120" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="121" spans="2:9">
@@ -5168,25 +5233,25 @@
         <v>5</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H121" s="1">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="122" spans="2:9">
@@ -5194,25 +5259,25 @@
         <v>5</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="H122" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="123" spans="2:9">
@@ -5220,25 +5285,25 @@
         <v>5</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H123" s="1">
         <v>4</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="124" spans="2:9">
@@ -5246,25 +5311,25 @@
         <v>5</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H124" s="1">
         <v>4</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="125" spans="2:9">
@@ -5272,25 +5337,25 @@
         <v>5</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="H125" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="126" spans="2:9">
@@ -5298,25 +5363,25 @@
         <v>5</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H126" s="1">
         <v>4</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="127" spans="2:9">
@@ -5324,25 +5389,25 @@
         <v>5</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H127" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="128" spans="2:9">
@@ -5350,25 +5415,25 @@
         <v>5</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="H128" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="129" spans="2:9">
@@ -5376,25 +5441,25 @@
         <v>5</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H129" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="130" spans="2:9">
@@ -5402,25 +5467,25 @@
         <v>5</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H130" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="131" spans="2:9">
@@ -5428,7 +5493,7 @@
         <v>5</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>51</v>
@@ -5437,16 +5502,16 @@
         <v>8</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H131" s="1">
         <v>4</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="132" spans="2:9">
@@ -5454,7 +5519,7 @@
         <v>5</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>51</v>
@@ -5463,16 +5528,16 @@
         <v>8</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H132" s="1">
         <v>4</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="133" spans="2:9">
@@ -5480,7 +5545,7 @@
         <v>5</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>51</v>
@@ -5489,16 +5554,16 @@
         <v>8</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H133" s="1">
         <v>4</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
     </row>
     <row r="134" spans="2:9">
@@ -5506,7 +5571,7 @@
         <v>5</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>51</v>
@@ -5515,16 +5580,16 @@
         <v>8</v>
       </c>
       <c r="F134" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G134" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G134" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="H134" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
     </row>
     <row r="135" spans="2:9">
@@ -5532,7 +5597,7 @@
         <v>5</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>51</v>
@@ -5541,16 +5606,16 @@
         <v>8</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H135" s="1">
         <v>4</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
     </row>
     <row r="136" spans="2:9">
@@ -5558,7 +5623,7 @@
         <v>5</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>51</v>
@@ -5567,16 +5632,16 @@
         <v>8</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H136" s="1">
         <v>4</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
     </row>
     <row r="137" spans="2:9">
@@ -5584,7 +5649,7 @@
         <v>5</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>51</v>
@@ -5593,16 +5658,16 @@
         <v>8</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="H137" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
     </row>
     <row r="138" spans="2:9">
@@ -5610,25 +5675,25 @@
         <v>5</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F138" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H138" s="1">
+        <v>4</v>
+      </c>
+      <c r="I138" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H138" s="1">
-        <v>4</v>
-      </c>
-      <c r="I138" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="139" spans="2:9">
@@ -5636,25 +5701,25 @@
         <v>5</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H139" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="140" spans="2:9">
@@ -5662,25 +5727,25 @@
         <v>5</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H140" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
     </row>
     <row r="141" spans="2:9">
@@ -5688,25 +5753,25 @@
         <v>5</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>133</v>
+        <v>77</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H141" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>148</v>
+        <v>78</v>
       </c>
     </row>
     <row r="142" spans="2:9">
@@ -5714,25 +5779,25 @@
         <v>5</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>135</v>
+        <v>66</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H142" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>136</v>
+        <v>67</v>
       </c>
     </row>
     <row r="143" spans="2:9">
@@ -5740,25 +5805,25 @@
         <v>5</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>137</v>
+        <v>58</v>
       </c>
       <c r="G143" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H143" s="1">
+        <v>4</v>
+      </c>
+      <c r="I143" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="H143" s="1">
-        <v>8</v>
-      </c>
-      <c r="I143" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="144" spans="2:9">
@@ -5766,25 +5831,25 @@
         <v>5</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H144" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
     </row>
     <row r="145" spans="2:9">
@@ -5792,25 +5857,25 @@
         <v>5</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H145" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="146" spans="2:9">
@@ -5818,25 +5883,25 @@
         <v>5</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H146" s="1">
         <v>8</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="147" spans="2:9">
@@ -5844,29 +5909,211 @@
         <v>5</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F147" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H147" s="1">
+        <v>5</v>
+      </c>
+      <c r="I147" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="148" spans="2:9">
+      <c r="B148" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H148" s="1">
+        <v>8</v>
+      </c>
+      <c r="I148" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="149" spans="2:9">
+      <c r="B149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H149" s="1">
+        <v>8</v>
+      </c>
+      <c r="I149" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="150" spans="2:9">
+      <c r="B150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H150" s="1">
+        <v>8</v>
+      </c>
+      <c r="I150" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="151" spans="2:9">
+      <c r="B151" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H151" s="1">
+        <v>8</v>
+      </c>
+      <c r="I151" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="152" spans="2:9">
+      <c r="B152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H152" s="1">
+        <v>8</v>
+      </c>
+      <c r="I152" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="153" spans="2:9">
+      <c r="B153" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F153" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G147" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H147" s="1">
-        <v>8</v>
-      </c>
-      <c r="I147" s="1" t="s">
+      <c r="G153" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H153" s="1">
+        <v>8</v>
+      </c>
+      <c r="I153" s="1" t="s">
         <v>146</v>
       </c>
     </row>
+    <row r="154" spans="2:9">
+      <c r="B154" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H154" s="1">
+        <v>8</v>
+      </c>
+      <c r="I154" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B2:I147">
+  <autoFilter ref="B2:I154">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>